<commit_message>
Updated the scripts and made all the functionalities working: chat bot left
</commit_message>
<xml_diff>
--- a/parsed_files/parsed_data.xlsx
+++ b/parsed_files/parsed_data.xlsx
@@ -10,9 +10,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_business_2023 (2)" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_business_2023_saving (1)" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_personal_2023 (1)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ebay" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="transaction_history-2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upwork_2023" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="transaction_history-2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upwork_2023" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18559,323 +18558,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>My Garage Order date:Apr 13, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Order date:Apr 09, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Order date:Apr 06, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Order date:Apr 06, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Order date:Apr 06, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Order date:Feb 19, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Order date:Feb 17, 2024 • Order total:</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Order total:</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Order date:Nov 20, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Order total:</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Order date:Nov 10, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Order date:Nov 10, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Order date:Nov 10, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Order date:Oct 24, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Order date:Oct 23, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Order date:Oct 15, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Order total:</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Order date:Aug 21, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Order date:Aug 07, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Order date:Apr 17, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Order date:Apr 12, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Order date:Apr 10, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Order date:Mar 02, 2023 • Order total:</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Uncategorized</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18988,7 +18670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>